<commit_message>
Sales order ,Employee bug fix
</commit_message>
<xml_diff>
--- a/RDDStaffPortal/RDDStaffPortal/Uploads/SalesOrder_Items.xlsx
+++ b/RDDStaffPortal/RDDStaffPortal/Uploads/SalesOrder_Items.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pramod - admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CD4951-8932-4BD2-B684-0D1BAC4B16B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8880"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -74,22 +75,16 @@
     <t>Epson L382 Printer</t>
   </si>
   <si>
-    <t>TZVATOUT</t>
-  </si>
-  <si>
     <t>TZSTZ01</t>
   </si>
   <si>
-    <t>C13T66444A</t>
-  </si>
-  <si>
-    <t>Epson T6644 70ml Yellow Ink Bottle</t>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,8 +94,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF1D1D1D"/>
+      <sz val="7"/>
+      <color rgb="FF2A2F5B"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -119,12 +114,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -134,7 +144,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,31 +426,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,47 +494,92 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
         <v>5</v>
       </c>
-      <c r="E2">
-        <v>25000</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>500</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>